<commit_message>
funciona extremadamente mal hago la copia por si puedo recuperar algo
</commit_message>
<xml_diff>
--- a/Claculos de desplazamiento.xlsx
+++ b/Claculos de desplazamiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Gonzalez\Google Drive\PROYECTOS\Nivelador-CNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C80E2B1-B071-41A6-BA9F-4CE68E0631B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC5E2AB-BE0F-4257-8836-AD6A28D90D11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7347841D-9F9A-4850-B4DB-E345D36E9524}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Vueltas</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>tics*Vuelta</t>
+  </si>
+  <si>
+    <t>Relacion motor</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>flancos encoder</t>
+  </si>
+  <si>
+    <t>Tics Vuelta</t>
   </si>
 </sst>
 </file>
@@ -491,7 +503,895 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tics*Vuelta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$4:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6288</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12576</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14672</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18864</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20960</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0433-4DD9-B675-6C44C0D37456}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="502500536"/>
+        <c:axId val="502501816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="502500536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="502501816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="502501816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="502500536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vueltas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-444E-430D-95C2-D1B1E27E077A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="508073272"/>
+        <c:axId val="508076472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="508073272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508076472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="508076472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508073272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1047,20 +1947,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1080,6 +3012,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF644B0D-2D76-4D9C-B2E1-54B9BA3DF7B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>623887</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>623887</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93FC67D1-AB70-4787-9F21-A2155CEBC6CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1385,14 +3389,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AB063C-6DBD-4514-BDA2-1898E9D3B4E3}">
-  <dimension ref="B3:D21"/>
+  <dimension ref="A3:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1526,7 +3532,36 @@
         <v>20960</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>131</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f>A19*B19*C19</f>
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2398</v>
       </c>

</xml_diff>

<commit_message>
funciona y translada de a 10 mm
</commit_message>
<xml_diff>
--- a/Claculos de desplazamiento.xlsx
+++ b/Claculos de desplazamiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Gonzalez\Google Drive\PROYECTOS\Nivelador-CNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC5E2AB-BE0F-4257-8836-AD6A28D90D11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A3C5F9-9B35-45DC-B4FF-8290E09077CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7347841D-9F9A-4850-B4DB-E345D36E9524}"/>
   </bookViews>
@@ -3389,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AB063C-6DBD-4514-BDA2-1898E9D3B4E3}">
-  <dimension ref="A3:D21"/>
+  <dimension ref="A3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3402,7 +3402,7 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>2096</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>4192</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>6288</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>8384</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>10480</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -3483,8 +3483,12 @@
         <f t="shared" si="0"/>
         <v>12576</v>
       </c>
+      <c r="M9">
+        <f>100*0.125</f>
+        <v>12.5</v>
+      </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -3496,7 +3500,7 @@
         <v>14672</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -3508,7 +3512,7 @@
         <v>16768</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -3520,7 +3524,7 @@
         <v>18864</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
funciona en el montaje se varia la constante a 0.666 esto para un dezplazamiento de 3 milimetros sobre 360 grados modificando el encoderpos
</commit_message>
<xml_diff>
--- a/Claculos de desplazamiento.xlsx
+++ b/Claculos de desplazamiento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Gonzalez\Google Drive\PROYECTOS\Nivelador-CNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A3C5F9-9B35-45DC-B4FF-8290E09077CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F0F48-1B19-45EF-99F2-05663EB0D55E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7347841D-9F9A-4850-B4DB-E345D36E9524}"/>
+    <workbookView xWindow="11070" yWindow="780" windowWidth="15375" windowHeight="7995" xr2:uid="{7347841D-9F9A-4850-B4DB-E345D36E9524}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -245,34 +245,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2096</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4192</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6288</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8384</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10480</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12576</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14672</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16768</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18864</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20960</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -284,34 +284,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>64</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,34 +642,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>64</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -681,34 +681,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2096</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4192</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6288</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8384</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10480</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12576</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14672</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16768</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18864</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20960</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1053,34 +1053,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>64</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3391,8 +3391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AB063C-6DBD-4514-BDA2-1898E9D3B4E3}">
   <dimension ref="A3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,10 +3418,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>2096</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -3429,11 +3429,11 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <f>$D$4*B5</f>
-        <v>4192</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -3441,11 +3441,11 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D13" si="0">$D$4*B6</f>
-        <v>6288</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -3453,11 +3453,11 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>8384</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -3465,11 +3465,11 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>10480</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -3477,11 +3477,11 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>12576</v>
+        <v>192</v>
       </c>
       <c r="M9">
         <f>100*0.125</f>
@@ -3493,11 +3493,11 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>14672</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -3505,11 +3505,11 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>16768</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -3517,11 +3517,11 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>18864</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -3529,11 +3529,11 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>20960</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>